<commit_message>
Approver Remarks & IsDomestic Function changed
</commit_message>
<xml_diff>
--- a/App_Templates/PrkBill_Template.xlsx
+++ b/App_Templates/PrkBill_Template.xlsx
@@ -22,30 +22,6 @@
     <author>lalit</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lalit:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DO NOT EDIT OR DELETE IN SYS.ID COLUMN</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B4" authorId="0">
       <text>
         <r>
@@ -566,7 +542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -849,6 +825,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1065,59 +1052,74 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="32" fillId="34" borderId="16" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="17" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="19" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="21" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="35" borderId="18" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="35" borderId="20" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="35" borderId="22" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="34" borderId="16" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="32" fillId="34" borderId="16" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="17" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="19" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="21" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="35" borderId="18" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="35" borderId="20" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="34" borderId="15" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="14" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="35" borderId="22" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="34" borderId="16" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="16" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="191">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1366,84 +1368,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>30481</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Right Brace 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2764156" y="57150"/>
-          <a:ext cx="198119" cy="390525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBrace">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" lIns="1944000" rtlCol="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DO NOT</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> DELETE OR EDIT</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1736,82 +1660,95 @@
   <dimension ref="A1:LQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="35" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="16" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
-    <col min="9" max="329" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="35" style="19" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="16" style="18" customWidth="1"/>
+    <col min="7" max="7" width="15" style="20" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="20" customWidth="1"/>
+    <col min="9" max="329" width="9.140625" style="3"/>
     <col min="330" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="13"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="G5" s="3">
+      <c r="G5" s="20">
         <v>0</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="20">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CF0D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
   <conditionalFormatting sqref="B4:B1048576">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
@@ -1837,7 +1774,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>